<commit_message>
Added Some Test Data
</commit_message>
<xml_diff>
--- a/SSUT/tesxtcel.xlsx
+++ b/SSUT/tesxtcel.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Personal\OpenXMLXLXSImporter\SSUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10E2733-62C6-4055-9429-F662F1F2AA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878D3544-DBC6-4E3B-B08A-A496EB4A4019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="4875" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="51480" yWindow="4875" windowWidth="29040" windowHeight="15840" xr2:uid="{3B186040-5F1E-4E49-AA34-01971BF76A73}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>A Header</t>
   </si>
@@ -85,6 +84,15 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Added Data Here</t>
+  </si>
+  <si>
+    <t>To Test</t>
+  </si>
+  <si>
+    <t>If I delete it</t>
   </si>
 </sst>
 </file>
@@ -419,34 +427,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.3984375" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" customWidth="1"/>
+    <col min="4" max="4" width="24.265625" customWidth="1"/>
+    <col min="5" max="5" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1328125" customWidth="1"/>
+    <col min="7" max="7" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.86328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -460,7 +465,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3">
+        <f>E7</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -498,7 +518,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>420</v>
       </c>
@@ -536,7 +556,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>69</v>
       </c>
@@ -578,7 +598,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>6.9</v>
       </c>
@@ -625,17 +645,14 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -643,7 +660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -651,7 +668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -660,7 +677,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
removed the test data
</commit_message>
<xml_diff>
--- a/SSUT/tesxtcel.xlsx
+++ b/SSUT/tesxtcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Personal\OpenXMLXLXSImporter\SSUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878D3544-DBC6-4E3B-B08A-A496EB4A4019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A82525-18A3-4FBC-8AB0-7B1EB026D515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>A Header</t>
   </si>
@@ -84,15 +84,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Added Data Here</t>
-  </si>
-  <si>
-    <t>To Test</t>
-  </si>
-  <si>
-    <t>If I delete it</t>
   </si>
 </sst>
 </file>
@@ -428,7 +419,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -466,19 +457,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3">
-        <f>E7</f>
-        <v>6</v>
-      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
hmm looks like we need to add a few more checks
</commit_message>
<xml_diff>
--- a/SSUT/tesxtcel.xlsx
+++ b/SSUT/tesxtcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Personal\OpenXMLXLSXImporter\SSUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5580CA7-14BD-4ED8-A42A-A985D6F899A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91669EE3-AD21-4ACF-8449-A84249FE3192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="4875" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>